<commit_message>
fix: fix some err and update dump db
</commit_message>
<xml_diff>
--- a/BetaCinema.ServerUI/Template/ImportTemplates/ShowtimeImport.xlsx
+++ b/BetaCinema.ServerUI/Template/ImportTemplates/ShowtimeImport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\blazor\BetaCinema\BetaCinema.ServerUI\Template\ImportTemplates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F6534E-E7D0-46AA-B45E-94A87A2B2942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7628CFEE-2718-4318-96A4-201A447B3A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>STT</t>
   </si>
@@ -38,12 +38,21 @@
   </si>
   <si>
     <t>Tên phim</t>
+  </si>
+  <si>
+    <t>Cún Cưng Đại Náo Nhà Hát</t>
+  </si>
+  <si>
+    <t>Beta Bắc Giang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -135,6 +144,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,7 +471,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -461,7 +479,7 @@
     <col min="1" max="1" width="4.21875" style="7" customWidth="1"/>
     <col min="2" max="2" width="40.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.44140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -491,7 +509,7 @@
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -502,10 +520,18 @@
       <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="10">
+        <v>45347.833333333336</v>
+      </c>
+      <c r="E4" s="4">
+        <v>40000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>